<commit_message>
Files from different tests
</commit_message>
<xml_diff>
--- a/tests/deployment_precision_test/precisiontest.xlsx
+++ b/tests/deployment_precision_test/precisiontest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Uni\HiWi\iobserve\Daten\deployment-experiments-migration-replication-allocation\deployment-experiments-migration-replication-allocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Uni\HiWi\iobserve\iobserve-analysis\tests\deployment_precision_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7571C4-5D22-4E92-B7C8-4D0ACBBC556B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12435" windowHeight="6570"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Migration</t>
   </si>
@@ -54,12 +55,15 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>Deallocation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,11 +444,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +556,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>